<commit_message>
rerun w/ default kapp of 339; FAL production was infeas.
</commit_message>
<xml_diff>
--- a/application/output_max_withoutMP_SC_RT_kapp_mapping/compiled_results.xlsx
+++ b/application/output_max_withoutMP_SC_RT_kapp_mapping/compiled_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG30"/>
+  <dimension ref="A1:AC30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -575,26 +575,6 @@
           <t>RBA: yield</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>yield on minimal media at 0.0% exp. growth</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>FBA: yield on minimal media at 0.0% exp. growth</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>RBA: yield on minimal media at 1.0% exp. growth</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>RBA: yield on minimal media at 0.0% exp. growth</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -616,25 +596,25 @@
         <v>76.09</v>
       </c>
       <c r="E2" t="n">
-        <v>17.81382212023962</v>
+        <v>17.81382211868642</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5695516930700739</v>
+        <v>0.5695516930204143</v>
       </c>
       <c r="G2" t="n">
         <v>-13.21</v>
       </c>
       <c r="H2" t="n">
-        <v>17.17010809154329</v>
+        <v>7.700839870852198</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5489705728353323</v>
+        <v>0.2462147851763999</v>
       </c>
       <c r="J2" t="n">
         <v>-13.21</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9638643507074793</v>
+        <v>0.4322957655883481</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
@@ -660,16 +640,12 @@
       </c>
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="n">
-        <v>17.17010809154329</v>
+        <v>7.700839870852198</v>
       </c>
       <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="n">
-        <v>0.5489705728353323</v>
-      </c>
-      <c r="AD2" t="inlineStr"/>
-      <c r="AE2" t="inlineStr"/>
-      <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="inlineStr"/>
+        <v>0.2462147851763999</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -691,25 +667,25 @@
         <v>122.16</v>
       </c>
       <c r="E3" t="n">
-        <v>2.555301936214222</v>
+        <v>2.555301938109797</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3122195089297514</v>
+        <v>0.3122195099690078</v>
       </c>
       <c r="G3" t="n">
-        <v>-5.549610217984472</v>
+        <v>-5.549610203628807</v>
       </c>
       <c r="H3" t="n">
-        <v>6.889254596904567</v>
+        <v>1.521111483573115</v>
       </c>
       <c r="I3" t="n">
-        <v>0.3536304962471257</v>
+        <v>0.07807976918502228</v>
       </c>
       <c r="J3" t="n">
         <v>-13.21</v>
       </c>
       <c r="K3" t="n">
-        <v>1.13263420809073</v>
+        <v>0.2500797249754597</v>
       </c>
       <c r="L3" t="n">
         <v>0.08</v>
@@ -737,16 +713,12 @@
       </c>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="n">
-        <v>6.889254596904567</v>
+        <v>1.521111483573115</v>
       </c>
       <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="n">
-        <v>0.3536304962471257</v>
-      </c>
-      <c r="AD3" t="inlineStr"/>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="inlineStr"/>
+        <v>0.07807976918502228</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -777,16 +749,16 @@
         <v>-5.545419566892341</v>
       </c>
       <c r="H4" t="n">
-        <v>18.72409243481652</v>
+        <v>2.853329673470618</v>
       </c>
       <c r="I4" t="n">
-        <v>0.7087247602369274</v>
+        <v>0.1080012500337344</v>
       </c>
       <c r="J4" t="n">
         <v>-13.21</v>
       </c>
       <c r="K4" t="n">
-        <v>1.065073059103834</v>
+        <v>0.1623045055206103</v>
       </c>
       <c r="L4" t="n">
         <v>0.13</v>
@@ -814,16 +786,12 @@
       </c>
       <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="n">
-        <v>18.72409243481652</v>
+        <v>2.853329673470618</v>
       </c>
       <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="n">
-        <v>0.7087247602369274</v>
-      </c>
-      <c r="AD4" t="inlineStr"/>
-      <c r="AE4" t="inlineStr"/>
-      <c r="AF4" t="inlineStr"/>
-      <c r="AG4" t="inlineStr"/>
+        <v>0.1080012500337344</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -845,25 +813,25 @@
         <v>90.08</v>
       </c>
       <c r="E5" t="n">
-        <v>8.29424549700787</v>
+        <v>8.294245457651009</v>
       </c>
       <c r="F5" t="n">
-        <v>0.747952115170689</v>
+        <v>0.7479521116177659</v>
       </c>
       <c r="G5" t="n">
-        <v>-5.544759808640229</v>
+        <v>-5.544759808668623</v>
       </c>
       <c r="H5" t="n">
-        <v>21.47203585549716</v>
+        <v>1.612555456519212</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8127370400708587</v>
+        <v>0.06103676230337551</v>
       </c>
       <c r="J5" t="n">
         <v>-13.21</v>
       </c>
       <c r="K5" t="n">
-        <v>1.086616407101657</v>
+        <v>0.08160517412185313</v>
       </c>
       <c r="L5" t="n">
         <v>0.14</v>
@@ -891,16 +859,12 @@
       </c>
       <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="n">
-        <v>21.47203585549716</v>
+        <v>1.612555456519212</v>
       </c>
       <c r="AB5" t="inlineStr"/>
       <c r="AC5" t="n">
-        <v>0.8127370400708587</v>
-      </c>
-      <c r="AD5" t="inlineStr"/>
-      <c r="AE5" t="inlineStr"/>
-      <c r="AF5" t="inlineStr"/>
-      <c r="AG5" t="inlineStr"/>
+        <v>0.06103676230337551</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -931,16 +895,16 @@
         <v>-5.545419566892341</v>
       </c>
       <c r="H6" t="n">
-        <v>18.72409243481652</v>
+        <v>2.853329673470618</v>
       </c>
       <c r="I6" t="n">
-        <v>0.7087247602369274</v>
+        <v>0.1080012500337344</v>
       </c>
       <c r="J6" t="n">
         <v>-13.21</v>
       </c>
       <c r="K6" t="n">
-        <v>1.065073059103834</v>
+        <v>0.1623045055206103</v>
       </c>
       <c r="L6" t="n">
         <v>0.13</v>
@@ -968,16 +932,12 @@
       </c>
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="n">
-        <v>18.72409243481652</v>
+        <v>2.853329673470618</v>
       </c>
       <c r="AB6" t="inlineStr"/>
       <c r="AC6" t="n">
-        <v>0.7087247602369274</v>
-      </c>
-      <c r="AD6" t="inlineStr"/>
-      <c r="AE6" t="inlineStr"/>
-      <c r="AF6" t="inlineStr"/>
-      <c r="AG6" t="inlineStr"/>
+        <v>0.1080012500337344</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -999,25 +959,25 @@
         <v>90.08</v>
       </c>
       <c r="E7" t="n">
-        <v>8.29424549700787</v>
+        <v>8.294245457651009</v>
       </c>
       <c r="F7" t="n">
-        <v>0.747952115170689</v>
+        <v>0.7479521116177659</v>
       </c>
       <c r="G7" t="n">
-        <v>-5.544759808640229</v>
+        <v>-5.544759808668623</v>
       </c>
       <c r="H7" t="n">
-        <v>21.47203585549716</v>
+        <v>1.612555456519212</v>
       </c>
       <c r="I7" t="n">
-        <v>0.8127370400708587</v>
+        <v>0.06103676230337551</v>
       </c>
       <c r="J7" t="n">
         <v>-13.21</v>
       </c>
       <c r="K7" t="n">
-        <v>1.086616407101657</v>
+        <v>0.08160517412185313</v>
       </c>
       <c r="L7" t="n">
         <v>0.14</v>
@@ -1045,16 +1005,12 @@
       </c>
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="n">
-        <v>21.47203585549716</v>
+        <v>1.612555456519212</v>
       </c>
       <c r="AB7" t="inlineStr"/>
       <c r="AC7" t="n">
-        <v>0.8127370400708587</v>
-      </c>
-      <c r="AD7" t="inlineStr"/>
-      <c r="AE7" t="inlineStr"/>
-      <c r="AF7" t="inlineStr"/>
-      <c r="AG7" t="inlineStr"/>
+        <v>0.06103676230337551</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1085,16 +1041,16 @@
         <v>-5.549441423005486</v>
       </c>
       <c r="H8" t="n">
-        <v>8.83155120575481</v>
+        <v>1.370104562450469</v>
       </c>
       <c r="I8" t="n">
-        <v>0.508808753089001</v>
+        <v>0.07893530567627992</v>
       </c>
       <c r="J8" t="n">
         <v>-13.21</v>
       </c>
       <c r="K8" t="n">
-        <v>1.105925987254771</v>
+        <v>0.1715705662084533</v>
       </c>
       <c r="L8" t="n">
         <v>0.07000000000000001</v>
@@ -1122,16 +1078,12 @@
       </c>
       <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="n">
-        <v>8.83155120575481</v>
+        <v>1.370104562450469</v>
       </c>
       <c r="AB8" t="inlineStr"/>
       <c r="AC8" t="n">
-        <v>0.508808753089001</v>
-      </c>
-      <c r="AD8" t="inlineStr"/>
-      <c r="AE8" t="inlineStr"/>
-      <c r="AF8" t="inlineStr"/>
-      <c r="AG8" t="inlineStr"/>
+        <v>0.07893530567627992</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1153,25 +1105,25 @@
         <v>234.33</v>
       </c>
       <c r="E9" t="n">
-        <v>2.844697655376326</v>
+        <v>2.844697655376308</v>
       </c>
       <c r="F9" t="n">
-        <v>0.280099580945372</v>
+        <v>0.2800995809453702</v>
       </c>
       <c r="G9" t="n">
         <v>-13.21</v>
       </c>
       <c r="H9" t="n">
-        <v>2.780971534486428</v>
+        <v>0.344335996115959</v>
       </c>
       <c r="I9" t="n">
-        <v>0.2738248685087798</v>
+        <v>0.03390461128064176</v>
       </c>
       <c r="J9" t="n">
         <v>-13.21</v>
       </c>
       <c r="K9" t="n">
-        <v>0.977598279813864</v>
+        <v>0.12104484828649</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
@@ -1197,16 +1149,12 @@
       </c>
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="n">
-        <v>2.780971534486428</v>
+        <v>0.344335996115959</v>
       </c>
       <c r="AB9" t="inlineStr"/>
       <c r="AC9" t="n">
-        <v>0.2738248685087798</v>
-      </c>
-      <c r="AD9" t="inlineStr"/>
-      <c r="AE9" t="inlineStr"/>
-      <c r="AF9" t="inlineStr"/>
-      <c r="AG9" t="inlineStr"/>
+        <v>0.03390461128064176</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1237,16 +1185,16 @@
         <v>-5.547686668594033</v>
       </c>
       <c r="H10" t="n">
-        <v>12.92858459956953</v>
+        <v>5.560921105611913</v>
       </c>
       <c r="I10" t="n">
-        <v>0.4895765599804274</v>
+        <v>0.210579634935342</v>
       </c>
       <c r="J10" t="n">
         <v>-13.21</v>
       </c>
       <c r="K10" t="n">
-        <v>1.084007491348663</v>
+        <v>0.466259867107411</v>
       </c>
       <c r="L10" t="n">
         <v>0.11</v>
@@ -1274,16 +1222,12 @@
       </c>
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="n">
-        <v>12.92858459956953</v>
+        <v>5.560921105611913</v>
       </c>
       <c r="AB10" t="inlineStr"/>
       <c r="AC10" t="n">
-        <v>0.4895765599804274</v>
-      </c>
-      <c r="AD10" t="inlineStr"/>
-      <c r="AE10" t="inlineStr"/>
-      <c r="AF10" t="inlineStr"/>
-      <c r="AG10" t="inlineStr"/>
+        <v>0.210579634935342</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1314,16 +1258,16 @@
         <v>-5.549820853802994</v>
       </c>
       <c r="H11" t="n">
-        <v>11.0726685589228</v>
+        <v>2.238988664816792</v>
       </c>
       <c r="I11" t="n">
-        <v>0.3448547105702764</v>
+        <v>0.06973258378201111</v>
       </c>
       <c r="J11" t="n">
         <v>-13.21</v>
       </c>
       <c r="K11" t="n">
-        <v>1.117741406250716</v>
+        <v>0.2260169105102519</v>
       </c>
       <c r="L11" t="n">
         <v>0.04</v>
@@ -1351,16 +1295,12 @@
       </c>
       <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="n">
-        <v>11.0726685589228</v>
+        <v>2.238988664816792</v>
       </c>
       <c r="AB11" t="inlineStr"/>
       <c r="AC11" t="n">
-        <v>0.3448547105702764</v>
-      </c>
-      <c r="AD11" t="inlineStr"/>
-      <c r="AE11" t="inlineStr"/>
-      <c r="AF11" t="inlineStr"/>
-      <c r="AG11" t="inlineStr"/>
+        <v>0.06973258378201111</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1382,25 +1322,25 @@
         <v>146.1</v>
       </c>
       <c r="E12" t="n">
-        <v>12.48937108880225</v>
+        <v>12.48937108880224</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7667243171293804</v>
+        <v>0.7667243171293799</v>
       </c>
       <c r="G12" t="n">
         <v>-13.21</v>
       </c>
       <c r="H12" t="n">
-        <v>12.97478395820177</v>
+        <v>1.843978700483669</v>
       </c>
       <c r="I12" t="n">
-        <v>0.7965238841508018</v>
+        <v>0.1132021220185437</v>
       </c>
       <c r="J12" t="n">
         <v>-13.21</v>
       </c>
       <c r="K12" t="n">
-        <v>1.038866077879193</v>
+        <v>0.1476438394994084</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
@@ -1426,16 +1366,12 @@
       </c>
       <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="n">
-        <v>12.97478395820177</v>
+        <v>1.843978700483669</v>
       </c>
       <c r="AB12" t="inlineStr"/>
       <c r="AC12" t="n">
-        <v>0.7965238841508018</v>
-      </c>
-      <c r="AD12" t="inlineStr"/>
-      <c r="AE12" t="inlineStr"/>
-      <c r="AF12" t="inlineStr"/>
-      <c r="AG12" t="inlineStr"/>
+        <v>0.1132021220185437</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1466,16 +1402,16 @@
         <v>-5.548570274707247</v>
       </c>
       <c r="H13" t="n">
-        <v>6.988885369853083</v>
+        <v>1.183900506283805</v>
       </c>
       <c r="I13" t="n">
-        <v>0.4791190590879487</v>
+        <v>0.08116162543904577</v>
       </c>
       <c r="J13" t="n">
         <v>-13.21</v>
       </c>
       <c r="K13" t="n">
-        <v>1.123937841548081</v>
+        <v>0.1903923886604355</v>
       </c>
       <c r="L13" t="n">
         <v>0.15</v>
@@ -1503,16 +1439,12 @@
       </c>
       <c r="Z13" t="inlineStr"/>
       <c r="AA13" t="n">
-        <v>6.988885369853083</v>
+        <v>1.183900506283805</v>
       </c>
       <c r="AB13" t="inlineStr"/>
       <c r="AC13" t="n">
-        <v>0.4791190590879487</v>
-      </c>
-      <c r="AD13" t="inlineStr"/>
-      <c r="AE13" t="inlineStr"/>
-      <c r="AF13" t="inlineStr"/>
-      <c r="AG13" t="inlineStr"/>
+        <v>0.08116162543904577</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1534,25 +1466,25 @@
         <v>256.4</v>
       </c>
       <c r="E14" t="n">
-        <v>1.016994536421366</v>
+        <v>1.016994536421386</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2607839207206942</v>
+        <v>0.2607839207206994</v>
       </c>
       <c r="G14" t="n">
         <v>-5.550180402242266</v>
       </c>
       <c r="H14" t="n">
-        <v>2.405626104262896</v>
+        <v>0.375845540667617</v>
       </c>
       <c r="I14" t="n">
-        <v>0.2591758910857484</v>
+        <v>0.04049261967207569</v>
       </c>
       <c r="J14" t="n">
         <v>-13.21</v>
       </c>
       <c r="K14" t="n">
-        <v>0.9938338620322068</v>
+        <v>0.1552726853717467</v>
       </c>
       <c r="L14" t="n">
         <v>0.1</v>
@@ -1580,16 +1512,12 @@
       </c>
       <c r="Z14" t="inlineStr"/>
       <c r="AA14" t="n">
-        <v>2.405626104262896</v>
+        <v>0.375845540667617</v>
       </c>
       <c r="AB14" t="inlineStr"/>
       <c r="AC14" t="n">
-        <v>0.2591758910857484</v>
-      </c>
-      <c r="AD14" t="inlineStr"/>
-      <c r="AE14" t="inlineStr"/>
-      <c r="AF14" t="inlineStr"/>
-      <c r="AG14" t="inlineStr"/>
+        <v>0.04049261967207569</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1620,16 +1548,16 @@
         <v>-5.550717505065815</v>
       </c>
       <c r="H15" t="n">
-        <v>2.34932219668753</v>
+        <v>0.399617466663044</v>
       </c>
       <c r="I15" t="n">
-        <v>0.2393289905603237</v>
+        <v>0.0407096332046705</v>
       </c>
       <c r="J15" t="n">
         <v>-13.21</v>
       </c>
       <c r="K15" t="n">
-        <v>0.9997281573106306</v>
+        <v>0.1700528067795393</v>
       </c>
       <c r="L15" t="n">
         <v>0.005</v>
@@ -1657,16 +1585,12 @@
       </c>
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="n">
-        <v>2.34932219668753</v>
+        <v>0.399617466663044</v>
       </c>
       <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="n">
-        <v>0.2393289905603237</v>
-      </c>
-      <c r="AD15" t="inlineStr"/>
-      <c r="AE15" t="inlineStr"/>
-      <c r="AF15" t="inlineStr"/>
-      <c r="AG15" t="inlineStr"/>
+        <v>0.0407096332046705</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1697,16 +1621,16 @@
         <v>-5.549184128068436</v>
       </c>
       <c r="H16" t="n">
-        <v>12.65142996893326</v>
+        <v>2.296940683351932</v>
       </c>
       <c r="I16" t="n">
-        <v>0.3940247282775204</v>
+        <v>0.07153748081045094</v>
       </c>
       <c r="J16" t="n">
         <v>-13.21</v>
       </c>
       <c r="K16" t="n">
-        <v>1.134034413231169</v>
+        <v>0.2058905425290388</v>
       </c>
       <c r="L16" t="n">
         <v>0.06</v>
@@ -1734,16 +1658,12 @@
       </c>
       <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="n">
-        <v>12.65142996893326</v>
+        <v>2.296940683351932</v>
       </c>
       <c r="AB16" t="inlineStr"/>
       <c r="AC16" t="n">
-        <v>0.3940247282775204</v>
-      </c>
-      <c r="AD16" t="inlineStr"/>
-      <c r="AE16" t="inlineStr"/>
-      <c r="AF16" t="inlineStr"/>
-      <c r="AG16" t="inlineStr"/>
+        <v>0.07153748081045094</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1765,25 +1685,25 @@
         <v>89.06999999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>8.860211568548351</v>
+        <v>8.860211623681527</v>
       </c>
       <c r="F17" t="n">
-        <v>0.7940334041382818</v>
+        <v>0.7940334091095929</v>
       </c>
       <c r="G17" t="n">
-        <v>-5.516810175723826</v>
+        <v>-5.516810175512664</v>
       </c>
       <c r="H17" t="n">
-        <v>24.41891984326444</v>
+        <v>23.31080656597566</v>
       </c>
       <c r="I17" t="n">
-        <v>0.9139161529935742</v>
+        <v>0.872443285644767</v>
       </c>
       <c r="J17" t="n">
         <v>-13.21</v>
       </c>
       <c r="K17" t="n">
-        <v>1.150979477979764</v>
+        <v>1.098748838066022</v>
       </c>
       <c r="L17" t="n">
         <v>0.6899999999999999</v>
@@ -1811,16 +1731,12 @@
       </c>
       <c r="Z17" t="inlineStr"/>
       <c r="AA17" t="n">
-        <v>24.41891984326444</v>
+        <v>23.31080656597566</v>
       </c>
       <c r="AB17" t="inlineStr"/>
       <c r="AC17" t="n">
-        <v>0.9139161529935742</v>
-      </c>
-      <c r="AD17" t="inlineStr"/>
-      <c r="AE17" t="inlineStr"/>
-      <c r="AF17" t="inlineStr"/>
-      <c r="AG17" t="inlineStr"/>
+        <v>0.872443285644767</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1842,25 +1758,25 @@
         <v>140.09</v>
       </c>
       <c r="E18" t="n">
-        <v>3.836460769542628</v>
+        <v>3.836460769542482</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5375941613289178</v>
+        <v>0.5375941613288975</v>
       </c>
       <c r="G18" t="n">
         <v>-5.5492542449107</v>
       </c>
       <c r="H18" t="n">
-        <v>10.29562896652916</v>
+        <v>1.562525293532522</v>
       </c>
       <c r="I18" t="n">
-        <v>0.6060500203049989</v>
+        <v>0.09197772073479249</v>
       </c>
       <c r="J18" t="n">
         <v>-13.21</v>
       </c>
       <c r="K18" t="n">
-        <v>1.127337430166392</v>
+        <v>0.1710913684542808</v>
       </c>
       <c r="L18" t="n">
         <v>0.07000000000000001</v>
@@ -1888,16 +1804,12 @@
       </c>
       <c r="Z18" t="inlineStr"/>
       <c r="AA18" t="n">
-        <v>10.29562896652916</v>
+        <v>1.562525293532522</v>
       </c>
       <c r="AB18" t="inlineStr"/>
       <c r="AC18" t="n">
-        <v>0.6060500203049989</v>
-      </c>
-      <c r="AD18" t="inlineStr"/>
-      <c r="AE18" t="inlineStr"/>
-      <c r="AF18" t="inlineStr"/>
-      <c r="AG18" t="inlineStr"/>
+        <v>0.09197772073479249</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1928,16 +1840,16 @@
         <v>-13.21</v>
       </c>
       <c r="H19" t="n">
-        <v>3.766640250683853</v>
+        <v>0.447192144312532</v>
       </c>
       <c r="I19" t="n">
-        <v>0.4308940361068346</v>
+        <v>0.05115764053737616</v>
       </c>
       <c r="J19" t="n">
         <v>-13.21</v>
       </c>
       <c r="K19" t="n">
-        <v>0.9489926833024327</v>
+        <v>0.112668597141941</v>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
@@ -1963,16 +1875,12 @@
       </c>
       <c r="Z19" t="inlineStr"/>
       <c r="AA19" t="n">
-        <v>3.766640250683853</v>
+        <v>0.447192144312532</v>
       </c>
       <c r="AB19" t="inlineStr"/>
       <c r="AC19" t="n">
-        <v>0.4308940361068346</v>
-      </c>
-      <c r="AD19" t="inlineStr"/>
-      <c r="AE19" t="inlineStr"/>
-      <c r="AF19" t="inlineStr"/>
-      <c r="AG19" t="inlineStr"/>
+        <v>0.05115764053737616</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2002,18 +1910,10 @@
       <c r="G20" t="n">
         <v>-0.332925</v>
       </c>
-      <c r="H20" t="n">
-        <v>0.10083907514254</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0.2375878909514378</v>
-      </c>
-      <c r="J20" t="n">
-        <v>-0.332925</v>
-      </c>
-      <c r="K20" t="n">
-        <v>1.00875753551832</v>
-      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr">
@@ -2031,35 +1931,15 @@
         </is>
       </c>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="n">
-        <v>0.135358218584754</v>
-      </c>
+      <c r="U20" t="inlineStr"/>
       <c r="V20" t="inlineStr"/>
-      <c r="W20" t="n">
-        <v>-0.332925</v>
-      </c>
+      <c r="W20" t="inlineStr"/>
       <c r="X20" t="inlineStr"/>
-      <c r="Y20" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="inlineStr"/>
-      <c r="AA20" t="n">
-        <v>0.10083907514254</v>
-      </c>
+      <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="inlineStr"/>
-      <c r="AC20" t="n">
-        <v>0.2375878909514378</v>
-      </c>
-      <c r="AD20" t="inlineStr"/>
-      <c r="AE20" t="n">
-        <v>0.135743300793755</v>
-      </c>
-      <c r="AF20" t="n">
-        <v>0.078150819418957</v>
-      </c>
-      <c r="AG20" t="n">
-        <v>0.08307504798705299</v>
-      </c>
+      <c r="AC20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2089,18 +1969,10 @@
       <c r="G21" t="n">
         <v>-0.332925</v>
       </c>
-      <c r="H21" t="n">
-        <v>0.114487601395357</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0.2435644445733376</v>
-      </c>
-      <c r="J21" t="n">
-        <v>-0.332925</v>
-      </c>
-      <c r="K21" t="n">
-        <v>1.002804814820772</v>
-      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr">
@@ -2114,35 +1986,15 @@
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
-      <c r="U21" t="n">
-        <v>0.148477553061659</v>
-      </c>
+      <c r="U21" t="inlineStr"/>
       <c r="V21" t="inlineStr"/>
-      <c r="W21" t="n">
-        <v>-0.332925</v>
-      </c>
+      <c r="W21" t="inlineStr"/>
       <c r="X21" t="inlineStr"/>
-      <c r="Y21" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="inlineStr"/>
-      <c r="AA21" t="n">
-        <v>0.114487601395357</v>
-      </c>
+      <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr"/>
-      <c r="AC21" t="n">
-        <v>0.2435644445733376</v>
-      </c>
-      <c r="AD21" t="inlineStr"/>
-      <c r="AE21" t="n">
-        <v>0.148839083264092</v>
-      </c>
-      <c r="AF21" t="n">
-        <v>0.079358646518538</v>
-      </c>
-      <c r="AG21" t="n">
-        <v>0.084589254540941</v>
-      </c>
+      <c r="AC21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2173,16 +2025,16 @@
         <v>-5.547262026771105</v>
       </c>
       <c r="H22" t="n">
-        <v>12.95352708331645</v>
+        <v>1.823872593359001</v>
       </c>
       <c r="I22" t="n">
-        <v>0.5611709158522057</v>
+        <v>0.07901355723656411</v>
       </c>
       <c r="J22" t="n">
         <v>-13.21</v>
       </c>
       <c r="K22" t="n">
-        <v>1.126988830996462</v>
+        <v>0.1586814177061871</v>
       </c>
       <c r="L22" t="n">
         <v>0.13</v>
@@ -2210,16 +2062,12 @@
       </c>
       <c r="Z22" t="inlineStr"/>
       <c r="AA22" t="n">
-        <v>12.95352708331645</v>
+        <v>1.823872593359001</v>
       </c>
       <c r="AB22" t="inlineStr"/>
       <c r="AC22" t="n">
-        <v>0.5611709158522057</v>
-      </c>
-      <c r="AD22" t="inlineStr"/>
-      <c r="AE22" t="inlineStr"/>
-      <c r="AF22" t="inlineStr"/>
-      <c r="AG22" t="inlineStr"/>
+        <v>0.07901355723656411</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2241,25 +2089,25 @@
         <v>329.4</v>
       </c>
       <c r="E23" t="n">
-        <v>2.511143874209327</v>
+        <v>2.511143874209235</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3475710873793104</v>
+        <v>0.3475710873792977</v>
       </c>
       <c r="G23" t="n">
         <v>-13.21</v>
       </c>
       <c r="H23" t="n">
-        <v>2.118149531018517</v>
+        <v>0.289478264146588</v>
       </c>
       <c r="I23" t="n">
-        <v>0.293176166960919</v>
+        <v>0.04006710888828895</v>
       </c>
       <c r="J23" t="n">
         <v>-13.21</v>
       </c>
       <c r="K23" t="n">
-        <v>0.8434998698294219</v>
+        <v>0.1152774506947538</v>
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
@@ -2285,16 +2133,12 @@
       </c>
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="n">
-        <v>2.118149531018517</v>
+        <v>0.289478264146588</v>
       </c>
       <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="n">
-        <v>0.293176166960919</v>
-      </c>
-      <c r="AD23" t="inlineStr"/>
-      <c r="AE23" t="inlineStr"/>
-      <c r="AF23" t="inlineStr"/>
-      <c r="AG23" t="inlineStr"/>
+        <v>0.04006710888828895</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2316,25 +2160,25 @@
         <v>228.24</v>
       </c>
       <c r="E24" t="n">
-        <v>1.465955758988984</v>
+        <v>1.465955758988985</v>
       </c>
       <c r="F24" t="n">
         <v>0.3345898405304263</v>
       </c>
       <c r="G24" t="n">
-        <v>-5.550743282537627</v>
+        <v>-5.55074328253763</v>
       </c>
       <c r="H24" t="n">
-        <v>3.766627938184681</v>
+        <v>0.447192144308166</v>
       </c>
       <c r="I24" t="n">
-        <v>0.3612375879550498</v>
+        <v>0.0428878599674444</v>
       </c>
       <c r="J24" t="n">
         <v>-13.21</v>
       </c>
       <c r="K24" t="n">
-        <v>1.079643026167139</v>
+        <v>0.1281804011127599</v>
       </c>
       <c r="L24" t="n">
         <v>0.0002</v>
@@ -2362,16 +2206,12 @@
       </c>
       <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="n">
-        <v>3.766627938184681</v>
+        <v>0.447192144308166</v>
       </c>
       <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="n">
-        <v>0.3612375879550498</v>
-      </c>
-      <c r="AD24" t="inlineStr"/>
-      <c r="AE24" t="inlineStr"/>
-      <c r="AF24" t="inlineStr"/>
-      <c r="AG24" t="inlineStr"/>
+        <v>0.0428878599674444</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2393,25 +2233,25 @@
         <v>246.3</v>
       </c>
       <c r="E25" t="n">
-        <v>1.116107088093233</v>
+        <v>1.11610708796343</v>
       </c>
       <c r="F25" t="n">
-        <v>0.2748980962445054</v>
+        <v>0.2748980962125331</v>
       </c>
       <c r="G25" t="n">
-        <v>-5.550726324289684</v>
+        <v>-5.550726324289716</v>
       </c>
       <c r="H25" t="n">
-        <v>2.867279814602072</v>
+        <v>0.328858739987122</v>
       </c>
       <c r="I25" t="n">
-        <v>0.2967446794393511</v>
+        <v>0.03403472548487591</v>
       </c>
       <c r="J25" t="n">
         <v>-13.21</v>
       </c>
       <c r="K25" t="n">
-        <v>1.07947156962271</v>
+        <v>0.1238085165150162</v>
       </c>
       <c r="L25" t="n">
         <v>0.003</v>
@@ -2439,16 +2279,12 @@
       </c>
       <c r="Z25" t="inlineStr"/>
       <c r="AA25" t="n">
-        <v>2.867279814602072</v>
+        <v>0.328858739987122</v>
       </c>
       <c r="AB25" t="inlineStr"/>
       <c r="AC25" t="n">
-        <v>0.2967446794393511</v>
-      </c>
-      <c r="AD25" t="inlineStr"/>
-      <c r="AE25" t="inlineStr"/>
-      <c r="AF25" t="inlineStr"/>
-      <c r="AG25" t="inlineStr"/>
+        <v>0.03403472548487591</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2470,25 +2306,25 @@
         <v>174.15</v>
       </c>
       <c r="E26" t="n">
-        <v>9.725652187360762</v>
+        <v>9.725652187360838</v>
       </c>
       <c r="F26" t="n">
-        <v>0.7116896739912114</v>
+        <v>0.7116896739912171</v>
       </c>
       <c r="G26" t="n">
         <v>-13.21</v>
       </c>
       <c r="H26" t="n">
-        <v>9.608810468778572</v>
+        <v>1.681231512630766</v>
       </c>
       <c r="I26" t="n">
-        <v>0.7031396001242478</v>
+        <v>0.1230267219182386</v>
       </c>
       <c r="J26" t="n">
         <v>-13.21</v>
       </c>
       <c r="K26" t="n">
-        <v>0.9879862330740109</v>
+        <v>0.1728656834773141</v>
       </c>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
@@ -2514,16 +2350,12 @@
       </c>
       <c r="Z26" t="inlineStr"/>
       <c r="AA26" t="n">
-        <v>9.608810468778572</v>
+        <v>1.681231512630766</v>
       </c>
       <c r="AB26" t="inlineStr"/>
       <c r="AC26" t="n">
-        <v>0.7031396001242478</v>
-      </c>
-      <c r="AD26" t="inlineStr"/>
-      <c r="AE26" t="inlineStr"/>
-      <c r="AF26" t="inlineStr"/>
-      <c r="AG26" t="inlineStr"/>
+        <v>0.1230267219182386</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2545,26 +2377,18 @@
         <v>270.5</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1013955884731691</v>
+        <v>0.1013955788142349</v>
       </c>
       <c r="F27" t="n">
-        <v>0.2406786063347258</v>
+        <v>0.2406785834077045</v>
       </c>
       <c r="G27" t="n">
         <v>-0.332925</v>
       </c>
-      <c r="H27" t="n">
-        <v>0.10222584280402</v>
-      </c>
-      <c r="I27" t="n">
-        <v>0.2426493474513912</v>
-      </c>
-      <c r="J27" t="n">
-        <v>-0.332925</v>
-      </c>
-      <c r="K27" t="n">
-        <v>1.008188268773356</v>
-      </c>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr">
@@ -2578,35 +2402,15 @@
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
-      <c r="U27" t="n">
-        <v>0.15276519020913</v>
-      </c>
+      <c r="U27" t="inlineStr"/>
       <c r="V27" t="inlineStr"/>
-      <c r="W27" t="n">
-        <v>-0.332925</v>
-      </c>
+      <c r="W27" t="inlineStr"/>
       <c r="X27" t="inlineStr"/>
-      <c r="Y27" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y27" t="inlineStr"/>
       <c r="Z27" t="inlineStr"/>
-      <c r="AA27" t="n">
-        <v>0.10222584280402</v>
-      </c>
+      <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="inlineStr"/>
-      <c r="AC27" t="n">
-        <v>0.2426493474513912</v>
-      </c>
-      <c r="AD27" t="inlineStr"/>
-      <c r="AE27" t="n">
-        <v>0.153175639705909</v>
-      </c>
-      <c r="AF27" t="n">
-        <v>0.078807086651177</v>
-      </c>
-      <c r="AG27" t="n">
-        <v>0.08371505342808699</v>
-      </c>
+      <c r="AC27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2628,25 +2432,25 @@
         <v>104.15</v>
       </c>
       <c r="E28" t="n">
-        <v>2.491549405834106</v>
+        <v>2.491549779661428</v>
       </c>
       <c r="F28" t="n">
-        <v>0.2594955171635242</v>
+        <v>0.2594955560978311</v>
       </c>
       <c r="G28" t="n">
-        <v>-5.550731080011727</v>
+        <v>-5.550731080009707</v>
       </c>
       <c r="H28" t="n">
-        <v>6.668894238641181</v>
+        <v>1.253099454693993</v>
       </c>
       <c r="I28" t="n">
-        <v>0.2918512488749464</v>
+        <v>0.05483947229180727</v>
       </c>
       <c r="J28" t="n">
         <v>-13.21</v>
       </c>
       <c r="K28" t="n">
-        <v>1.124687054578414</v>
+        <v>0.2113310652269225</v>
       </c>
       <c r="L28" t="n">
         <v>0.001</v>
@@ -2674,16 +2478,12 @@
       </c>
       <c r="Z28" t="inlineStr"/>
       <c r="AA28" t="n">
-        <v>6.668894238641181</v>
+        <v>1.253099454693993</v>
       </c>
       <c r="AB28" t="inlineStr"/>
       <c r="AC28" t="n">
-        <v>0.2918512488749464</v>
-      </c>
-      <c r="AD28" t="inlineStr"/>
-      <c r="AE28" t="inlineStr"/>
-      <c r="AF28" t="inlineStr"/>
-      <c r="AG28" t="inlineStr"/>
+        <v>0.05483947229180727</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2705,25 +2505,25 @@
         <v>824.3</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1308423257890941</v>
+        <v>0.1308423337395128</v>
       </c>
       <c r="F29" t="n">
-        <v>0.2719810746481115</v>
+        <v>0.2719810911745942</v>
       </c>
       <c r="G29" t="n">
         <v>-2.20113372715757</v>
       </c>
       <c r="H29" t="n">
-        <v>0.128805203044783</v>
+        <v>0.009197509411190999</v>
       </c>
       <c r="I29" t="n">
-        <v>0.2677465211131878</v>
+        <v>0.01911880179945834</v>
       </c>
       <c r="J29" t="n">
         <v>-2.201133727157571</v>
       </c>
       <c r="K29" t="n">
-        <v>0.9844307051863722</v>
+        <v>0.07029459921971307</v>
       </c>
       <c r="L29" t="n">
         <v>0.14</v>
@@ -2755,16 +2555,12 @@
       </c>
       <c r="Z29" t="inlineStr"/>
       <c r="AA29" t="n">
-        <v>0.128805203044783</v>
+        <v>0.009197509411190999</v>
       </c>
       <c r="AB29" t="inlineStr"/>
       <c r="AC29" t="n">
-        <v>0.2677465211131878</v>
-      </c>
-      <c r="AD29" t="inlineStr"/>
-      <c r="AE29" t="inlineStr"/>
-      <c r="AF29" t="inlineStr"/>
-      <c r="AG29" t="inlineStr"/>
+        <v>0.01911880179945834</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2820,10 +2616,6 @@
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="inlineStr"/>
       <c r="AC30" t="inlineStr"/>
-      <c r="AD30" t="inlineStr"/>
-      <c r="AE30" t="inlineStr"/>
-      <c r="AF30" t="inlineStr"/>
-      <c r="AG30" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
rerun; kapp calculations now output separate file for used rxns w/o default kapps
</commit_message>
<xml_diff>
--- a/application/output_max_withoutMP_SC_RT_kapp_mapping/compiled_results.xlsx
+++ b/application/output_max_withoutMP_SC_RT_kapp_mapping/compiled_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC30"/>
+  <dimension ref="A1:AG30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -575,6 +575,26 @@
           <t>RBA: yield</t>
         </is>
       </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>yield on minimal media at 0.0% exp. growth</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>FBA: yield on minimal media at 0.0% exp. growth</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>RBA: yield on minimal media at 1.0% exp. growth</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>RBA: yield on minimal media at 0.0% exp. growth</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -596,25 +616,25 @@
         <v>76.09</v>
       </c>
       <c r="E2" t="n">
-        <v>17.81382211868638</v>
+        <v>17.81382211868675</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5695516930204129</v>
+        <v>0.5695516930204249</v>
       </c>
       <c r="G2" t="n">
         <v>-13.21</v>
       </c>
       <c r="H2" t="n">
-        <v>7.756955448095802</v>
+        <v>17.3386072585456</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2480089381555287</v>
+        <v>0.5543579055031499</v>
       </c>
       <c r="J2" t="n">
         <v>-13.21</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4354458799697397</v>
+        <v>0.9733232510701534</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
@@ -640,12 +660,16 @@
       </c>
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="n">
-        <v>7.756955448095802</v>
+        <v>17.3386072585456</v>
       </c>
       <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="n">
-        <v>0.2480089381555287</v>
-      </c>
+        <v>0.5543579055031499</v>
+      </c>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -676,16 +700,16 @@
         <v>-5.549610203628807</v>
       </c>
       <c r="H3" t="n">
-        <v>2.36613078072119</v>
+        <v>6.945532124342357</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1214552300836712</v>
+        <v>0.3565192630469954</v>
       </c>
       <c r="J3" t="n">
         <v>-13.21</v>
       </c>
       <c r="K3" t="n">
-        <v>0.3890058955499844</v>
+        <v>1.141886562701943</v>
       </c>
       <c r="L3" t="n">
         <v>0.08</v>
@@ -713,12 +737,16 @@
       </c>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="n">
-        <v>2.36613078072119</v>
+        <v>6.945532124342357</v>
       </c>
       <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="n">
-        <v>0.1214552300836712</v>
-      </c>
+        <v>0.3565192630469954</v>
+      </c>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -740,25 +768,25 @@
         <v>90.08</v>
       </c>
       <c r="E4" t="n">
-        <v>7.379942361103544</v>
+        <v>7.379942359355508</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6654236103138855</v>
+        <v>0.6654236101561112</v>
       </c>
       <c r="G4" t="n">
-        <v>-5.545419566892341</v>
+        <v>-5.545419566893675</v>
       </c>
       <c r="H4" t="n">
-        <v>2.913915633067646</v>
+        <v>19.35580242320651</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1102944863995882</v>
+        <v>0.7326355859081614</v>
       </c>
       <c r="J4" t="n">
         <v>-13.21</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1657507859505637</v>
+        <v>1.101006298433387</v>
       </c>
       <c r="L4" t="n">
         <v>0.13</v>
@@ -786,12 +814,16 @@
       </c>
       <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="n">
-        <v>2.913915633067646</v>
+        <v>19.35580242320651</v>
       </c>
       <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="n">
-        <v>0.1102944863995882</v>
-      </c>
+        <v>0.7326355859081614</v>
+      </c>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -813,25 +845,25 @@
         <v>90.08</v>
       </c>
       <c r="E5" t="n">
-        <v>8.294245459149213</v>
+        <v>8.294244088547805</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7479521117530147</v>
+        <v>0.7479519880225586</v>
       </c>
       <c r="G5" t="n">
-        <v>-5.544759808667549</v>
+        <v>-5.54475980965657</v>
       </c>
       <c r="H5" t="n">
-        <v>2.438357979395267</v>
+        <v>21.7221718902911</v>
       </c>
       <c r="I5" t="n">
-        <v>0.09229417555669334</v>
+        <v>0.8222049276014879</v>
       </c>
       <c r="J5" t="n">
         <v>-13.21</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1233958352499047</v>
+        <v>1.099275007979108</v>
       </c>
       <c r="L5" t="n">
         <v>0.14</v>
@@ -859,12 +891,16 @@
       </c>
       <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="n">
-        <v>2.438357979395267</v>
+        <v>21.7221718902911</v>
       </c>
       <c r="AB5" t="inlineStr"/>
       <c r="AC5" t="n">
-        <v>0.09229417555669334</v>
-      </c>
+        <v>0.8222049276014879</v>
+      </c>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -886,25 +922,25 @@
         <v>90.08</v>
       </c>
       <c r="E6" t="n">
-        <v>7.379942361103544</v>
+        <v>7.379942359355508</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6654236103138855</v>
+        <v>0.6654236101561112</v>
       </c>
       <c r="G6" t="n">
-        <v>-5.545419566892341</v>
+        <v>-5.545419566893675</v>
       </c>
       <c r="H6" t="n">
-        <v>2.913915633067646</v>
+        <v>19.35580242320651</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1102944863995882</v>
+        <v>0.7326355859081614</v>
       </c>
       <c r="J6" t="n">
         <v>-13.21</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1657507859505637</v>
+        <v>1.101006298433387</v>
       </c>
       <c r="L6" t="n">
         <v>0.13</v>
@@ -932,12 +968,16 @@
       </c>
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="n">
-        <v>2.913915633067646</v>
+        <v>19.35580242320651</v>
       </c>
       <c r="AB6" t="inlineStr"/>
       <c r="AC6" t="n">
-        <v>0.1102944863995882</v>
-      </c>
+        <v>0.7326355859081614</v>
+      </c>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -959,25 +999,25 @@
         <v>90.08</v>
       </c>
       <c r="E7" t="n">
-        <v>8.294245459149213</v>
+        <v>8.294244088547805</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7479521117530147</v>
+        <v>0.7479519880225586</v>
       </c>
       <c r="G7" t="n">
-        <v>-5.544759808667549</v>
+        <v>-5.54475980965657</v>
       </c>
       <c r="H7" t="n">
-        <v>2.438357979395267</v>
+        <v>21.7221718902911</v>
       </c>
       <c r="I7" t="n">
-        <v>0.09229417555669334</v>
+        <v>0.8222049276014879</v>
       </c>
       <c r="J7" t="n">
         <v>-13.21</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1233958352499047</v>
+        <v>1.099275007979108</v>
       </c>
       <c r="L7" t="n">
         <v>0.14</v>
@@ -1005,12 +1045,16 @@
       </c>
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="n">
-        <v>2.438357979395267</v>
+        <v>21.7221718902911</v>
       </c>
       <c r="AB7" t="inlineStr"/>
       <c r="AC7" t="n">
-        <v>0.09229417555669334</v>
-      </c>
+        <v>0.8222049276014879</v>
+      </c>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1032,25 +1076,25 @@
         <v>137.11</v>
       </c>
       <c r="E8" t="n">
-        <v>3.354728528907348</v>
+        <v>3.354728528907292</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4600748684385474</v>
+        <v>0.4600748684385398</v>
       </c>
       <c r="G8" t="n">
-        <v>-5.549441423005487</v>
+        <v>-5.549441423005486</v>
       </c>
       <c r="H8" t="n">
-        <v>2.051648440349357</v>
+        <v>8.209980036982234</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1182008302268492</v>
+        <v>0.4729984130965015</v>
       </c>
       <c r="J8" t="n">
         <v>-13.21</v>
       </c>
       <c r="K8" t="n">
-        <v>0.2569165114973834</v>
+        <v>1.028090090427724</v>
       </c>
       <c r="L8" t="n">
         <v>0.07000000000000001</v>
@@ -1078,12 +1122,16 @@
       </c>
       <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="n">
-        <v>2.051648440349357</v>
+        <v>8.209980036982234</v>
       </c>
       <c r="AB8" t="inlineStr"/>
       <c r="AC8" t="n">
-        <v>0.1182008302268492</v>
-      </c>
+        <v>0.4729984130965015</v>
+      </c>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1105,25 +1153,25 @@
         <v>234.33</v>
       </c>
       <c r="E9" t="n">
-        <v>2.844697655376507</v>
+        <v>2.844697655376317</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2800995809453898</v>
+        <v>0.2800995809453711</v>
       </c>
       <c r="G9" t="n">
         <v>-13.21</v>
       </c>
       <c r="H9" t="n">
-        <v>0.351055197241386</v>
+        <v>2.727231542311549</v>
       </c>
       <c r="I9" t="n">
-        <v>0.03456620897836644</v>
+        <v>0.2685334276908979</v>
       </c>
       <c r="J9" t="n">
         <v>-13.21</v>
       </c>
       <c r="K9" t="n">
-        <v>0.1234068571673648</v>
+        <v>0.9587069955069693</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
@@ -1149,12 +1197,16 @@
       </c>
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="n">
-        <v>0.351055197241386</v>
+        <v>2.727231542311549</v>
       </c>
       <c r="AB9" t="inlineStr"/>
       <c r="AC9" t="n">
-        <v>0.03456620897836644</v>
-      </c>
+        <v>0.2685334276908979</v>
+      </c>
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1176,25 +1228,25 @@
         <v>90.12</v>
       </c>
       <c r="E10" t="n">
-        <v>5.008732116108107</v>
+        <v>5.008732115512615</v>
       </c>
       <c r="F10" t="n">
-        <v>0.4516357717891071</v>
+        <v>0.4516357717353817</v>
       </c>
       <c r="G10" t="n">
-        <v>-5.547686668594033</v>
+        <v>-5.547686668594402</v>
       </c>
       <c r="H10" t="n">
-        <v>5.648164340856276</v>
+        <v>12.86836716697117</v>
       </c>
       <c r="I10" t="n">
-        <v>0.2138833409724221</v>
+        <v>0.4872962605961205</v>
       </c>
       <c r="J10" t="n">
         <v>-13.21</v>
       </c>
       <c r="K10" t="n">
-        <v>0.4735748457770429</v>
+        <v>1.078958512793873</v>
       </c>
       <c r="L10" t="n">
         <v>0.11</v>
@@ -1222,12 +1274,16 @@
       </c>
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="n">
-        <v>5.648164340856276</v>
+        <v>12.86836716697117</v>
       </c>
       <c r="AB10" t="inlineStr"/>
       <c r="AC10" t="n">
-        <v>0.2138833409724221</v>
-      </c>
+        <v>0.4872962605961205</v>
+      </c>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1249,25 +1305,25 @@
         <v>74.12</v>
       </c>
       <c r="E11" t="n">
-        <v>4.161856554711804</v>
+        <v>4.161856555785772</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3085281698346767</v>
+        <v>0.3085281699143055</v>
       </c>
       <c r="G11" t="n">
-        <v>-5.54982085380343</v>
+        <v>-5.549820853803196</v>
       </c>
       <c r="H11" t="n">
-        <v>2.275535382984859</v>
+        <v>11.19104235383226</v>
       </c>
       <c r="I11" t="n">
-        <v>0.07087081959653714</v>
+        <v>0.3485414244428515</v>
       </c>
       <c r="J11" t="n">
         <v>-13.21</v>
       </c>
       <c r="K11" t="n">
-        <v>0.2297061549825836</v>
+        <v>1.1296907654807</v>
       </c>
       <c r="L11" t="n">
         <v>0.04</v>
@@ -1295,12 +1351,16 @@
       </c>
       <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="n">
-        <v>2.275535382984859</v>
+        <v>11.19104235383226</v>
       </c>
       <c r="AB11" t="inlineStr"/>
       <c r="AC11" t="n">
-        <v>0.07087081959653714</v>
-      </c>
+        <v>0.3485414244428515</v>
+      </c>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1331,16 +1391,16 @@
         <v>-13.21</v>
       </c>
       <c r="H12" t="n">
-        <v>1.874347601810321</v>
+        <v>13.01766641721771</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1150664733110217</v>
+        <v>0.7991564445793493</v>
       </c>
       <c r="J12" t="n">
         <v>-13.21</v>
       </c>
       <c r="K12" t="n">
-        <v>0.1500754192091259</v>
+        <v>1.04229959416365</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
@@ -1366,12 +1426,16 @@
       </c>
       <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="n">
-        <v>1.874347601810321</v>
+        <v>13.01766641721771</v>
       </c>
       <c r="AB12" t="inlineStr"/>
       <c r="AC12" t="n">
-        <v>0.1150664733110217</v>
-      </c>
+        <v>0.7991564445793493</v>
+      </c>
+      <c r="AD12" t="inlineStr"/>
+      <c r="AE12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1393,25 +1457,25 @@
         <v>163.15</v>
       </c>
       <c r="E13" t="n">
-        <v>2.611823932281903</v>
+        <v>2.611823947915461</v>
       </c>
       <c r="F13" t="n">
-        <v>0.4262860821805085</v>
+        <v>0.4262860847331228</v>
       </c>
       <c r="G13" t="n">
-        <v>-5.548570274707237</v>
+        <v>-5.548570274694224</v>
       </c>
       <c r="H13" t="n">
-        <v>1.667994984854537</v>
+        <v>7.064049293642649</v>
       </c>
       <c r="I13" t="n">
-        <v>0.1143484469146076</v>
+        <v>0.4842718791068256</v>
       </c>
       <c r="J13" t="n">
         <v>-13.21</v>
       </c>
       <c r="K13" t="n">
-        <v>0.2682434442374954</v>
+        <v>1.13602553883504</v>
       </c>
       <c r="L13" t="n">
         <v>0.15</v>
@@ -1439,12 +1503,16 @@
       </c>
       <c r="Z13" t="inlineStr"/>
       <c r="AA13" t="n">
-        <v>1.667994984854537</v>
+        <v>7.064049293642649</v>
       </c>
       <c r="AB13" t="inlineStr"/>
       <c r="AC13" t="n">
-        <v>0.1143484469146076</v>
-      </c>
+        <v>0.4842718791068256</v>
+      </c>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1475,16 +1543,16 @@
         <v>-5.550180402242267</v>
       </c>
       <c r="H14" t="n">
-        <v>0.390772400735024</v>
+        <v>2.47037636942488</v>
       </c>
       <c r="I14" t="n">
-        <v>0.04210080069913844</v>
+        <v>0.2661519160140021</v>
       </c>
       <c r="J14" t="n">
         <v>-13.21</v>
       </c>
       <c r="K14" t="n">
-        <v>0.1614394038665762</v>
+        <v>1.020584073122554</v>
       </c>
       <c r="L14" t="n">
         <v>0.1</v>
@@ -1512,12 +1580,16 @@
       </c>
       <c r="Z14" t="inlineStr"/>
       <c r="AA14" t="n">
-        <v>0.390772400735024</v>
+        <v>2.47037636942488</v>
       </c>
       <c r="AB14" t="inlineStr"/>
       <c r="AC14" t="n">
-        <v>0.04210080069913844</v>
-      </c>
+        <v>0.2661519160140021</v>
+      </c>
+      <c r="AD14" t="inlineStr"/>
+      <c r="AE14" t="inlineStr"/>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1548,16 +1620,16 @@
         <v>-5.550717505065815</v>
       </c>
       <c r="H15" t="n">
-        <v>0.415952454023202</v>
+        <v>2.408573268556511</v>
       </c>
       <c r="I15" t="n">
-        <v>0.04237370296965823</v>
+        <v>0.2453649864914116</v>
       </c>
       <c r="J15" t="n">
         <v>-13.21</v>
       </c>
       <c r="K15" t="n">
-        <v>0.177003980542035</v>
+        <v>1.024941797645607</v>
       </c>
       <c r="L15" t="n">
         <v>0.005</v>
@@ -1585,12 +1657,16 @@
       </c>
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="n">
-        <v>0.415952454023202</v>
+        <v>2.408573268556511</v>
       </c>
       <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="n">
-        <v>0.04237370296965823</v>
-      </c>
+        <v>0.2453649864914116</v>
+      </c>
+      <c r="AD15" t="inlineStr"/>
+      <c r="AE15" t="inlineStr"/>
+      <c r="AF15" t="inlineStr"/>
+      <c r="AG15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1612,25 +1688,25 @@
         <v>74.12</v>
       </c>
       <c r="E16" t="n">
-        <v>4.686402963931311</v>
+        <v>4.686403727429883</v>
       </c>
       <c r="F16" t="n">
-        <v>0.347453886221922</v>
+        <v>0.3474539428442743</v>
       </c>
       <c r="G16" t="n">
-        <v>-5.549184128323032</v>
+        <v>-5.549184128068751</v>
       </c>
       <c r="H16" t="n">
-        <v>12.62906481237367</v>
+        <v>12.6797430372781</v>
       </c>
       <c r="I16" t="n">
-        <v>0.3933281726503767</v>
+        <v>0.3949065297093487</v>
       </c>
       <c r="J16" t="n">
         <v>-13.21</v>
       </c>
       <c r="K16" t="n">
-        <v>1.132029855608391</v>
+        <v>1.136572307905403</v>
       </c>
       <c r="L16" t="n">
         <v>0.06</v>
@@ -1658,12 +1734,16 @@
       </c>
       <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="n">
-        <v>12.62906481237367</v>
+        <v>12.6797430372781</v>
       </c>
       <c r="AB16" t="inlineStr"/>
       <c r="AC16" t="n">
-        <v>0.3933281726503767</v>
-      </c>
+        <v>0.3949065297093487</v>
+      </c>
+      <c r="AD16" t="inlineStr"/>
+      <c r="AE16" t="inlineStr"/>
+      <c r="AF16" t="inlineStr"/>
+      <c r="AG16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1694,16 +1774,16 @@
         <v>-5.516810175715775</v>
       </c>
       <c r="H17" t="n">
-        <v>23.76814489072392</v>
+        <v>24.49618034866554</v>
       </c>
       <c r="I17" t="n">
-        <v>0.8895598856030466</v>
+        <v>0.9168077478850649</v>
       </c>
       <c r="J17" t="n">
         <v>-13.21</v>
       </c>
       <c r="K17" t="n">
-        <v>1.120305368457943</v>
+        <v>1.154621131665783</v>
       </c>
       <c r="L17" t="n">
         <v>0.6899999999999999</v>
@@ -1731,12 +1811,16 @@
       </c>
       <c r="Z17" t="inlineStr"/>
       <c r="AA17" t="n">
-        <v>23.76814489072392</v>
+        <v>24.49618034866554</v>
       </c>
       <c r="AB17" t="inlineStr"/>
       <c r="AC17" t="n">
-        <v>0.8895598856030466</v>
-      </c>
+        <v>0.9168077478850649</v>
+      </c>
+      <c r="AD17" t="inlineStr"/>
+      <c r="AE17" t="inlineStr"/>
+      <c r="AF17" t="inlineStr"/>
+      <c r="AG17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1758,25 +1842,25 @@
         <v>140.09</v>
       </c>
       <c r="E18" t="n">
-        <v>3.836460793415273</v>
+        <v>3.836460769542511</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5375941646750338</v>
+        <v>0.5375941613289015</v>
       </c>
       <c r="G18" t="n">
-        <v>-5.549254244901423</v>
+        <v>-5.5492542449107</v>
       </c>
       <c r="H18" t="n">
-        <v>2.510682308742037</v>
+        <v>10.40365748164947</v>
       </c>
       <c r="I18" t="n">
-        <v>0.1477907827816246</v>
+        <v>0.6124090959860503</v>
       </c>
       <c r="J18" t="n">
         <v>-13.21</v>
       </c>
       <c r="K18" t="n">
-        <v>0.2749114341130571</v>
+        <v>1.139166196433776</v>
       </c>
       <c r="L18" t="n">
         <v>0.07000000000000001</v>
@@ -1804,12 +1888,16 @@
       </c>
       <c r="Z18" t="inlineStr"/>
       <c r="AA18" t="n">
-        <v>2.510682308742037</v>
+        <v>10.40365748164947</v>
       </c>
       <c r="AB18" t="inlineStr"/>
       <c r="AC18" t="n">
-        <v>0.1477907827816246</v>
-      </c>
+        <v>0.6124090959860503</v>
+      </c>
+      <c r="AD18" t="inlineStr"/>
+      <c r="AE18" t="inlineStr"/>
+      <c r="AF18" t="inlineStr"/>
+      <c r="AG18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1831,25 +1919,25 @@
         <v>272.25</v>
       </c>
       <c r="E19" t="n">
-        <v>3.969093036182585</v>
+        <v>3.969093036182524</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4540541183177073</v>
+        <v>0.4540541183177003</v>
       </c>
       <c r="G19" t="n">
         <v>-13.21</v>
       </c>
       <c r="H19" t="n">
-        <v>0.509380836303288</v>
+        <v>3.857840565265874</v>
       </c>
       <c r="I19" t="n">
-        <v>0.05827186825987675</v>
+        <v>0.4413271194461117</v>
       </c>
       <c r="J19" t="n">
         <v>-13.21</v>
       </c>
       <c r="K19" t="n">
-        <v>0.1283368345513017</v>
+        <v>0.9719703040713673</v>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
@@ -1875,12 +1963,16 @@
       </c>
       <c r="Z19" t="inlineStr"/>
       <c r="AA19" t="n">
-        <v>0.509380836303288</v>
+        <v>3.857840565265874</v>
       </c>
       <c r="AB19" t="inlineStr"/>
       <c r="AC19" t="n">
-        <v>0.05827186825987675</v>
-      </c>
+        <v>0.4413271194461117</v>
+      </c>
+      <c r="AD19" t="inlineStr"/>
+      <c r="AE19" t="inlineStr"/>
+      <c r="AF19" t="inlineStr"/>
+      <c r="AG19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1910,10 +2002,18 @@
       <c r="G20" t="n">
         <v>-0.332925</v>
       </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
+      <c r="H20" t="n">
+        <v>0.100346185993871</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.2364265902042861</v>
+      </c>
+      <c r="J20" t="n">
+        <v>-0.332925</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1.003826851235544</v>
+      </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr">
@@ -1931,15 +2031,35 @@
         </is>
       </c>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
+      <c r="U20" t="n">
+        <v>0.135358218584754</v>
+      </c>
       <c r="V20" t="inlineStr"/>
-      <c r="W20" t="inlineStr"/>
+      <c r="W20" t="n">
+        <v>-0.332925</v>
+      </c>
       <c r="X20" t="inlineStr"/>
-      <c r="Y20" t="inlineStr"/>
+      <c r="Y20" t="n">
+        <v>0</v>
+      </c>
       <c r="Z20" t="inlineStr"/>
-      <c r="AA20" t="inlineStr"/>
+      <c r="AA20" t="n">
+        <v>0.100346185993871</v>
+      </c>
       <c r="AB20" t="inlineStr"/>
-      <c r="AC20" t="inlineStr"/>
+      <c r="AC20" t="n">
+        <v>0.2364265902042861</v>
+      </c>
+      <c r="AD20" t="inlineStr"/>
+      <c r="AE20" t="n">
+        <v>0.135743300793755</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>0.078150819418957</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>0.08307504798705299</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1961,18 +2081,26 @@
         <v>242.44</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1141673721518172</v>
+        <v>0.1141673830273941</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2428831790311451</v>
+        <v>0.2428832021681819</v>
       </c>
       <c r="G21" t="n">
         <v>-0.332925</v>
       </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
+      <c r="H21" t="n">
+        <v>0.114485813726807</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.2435606414322798</v>
+      </c>
+      <c r="J21" t="n">
+        <v>-0.332925</v>
+      </c>
+      <c r="K21" t="n">
+        <v>1.002789156508357</v>
+      </c>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr">
@@ -1986,15 +2114,35 @@
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr"/>
+      <c r="U21" t="n">
+        <v>0.148477553061659</v>
+      </c>
       <c r="V21" t="inlineStr"/>
-      <c r="W21" t="inlineStr"/>
+      <c r="W21" t="n">
+        <v>-0.332925</v>
+      </c>
       <c r="X21" t="inlineStr"/>
-      <c r="Y21" t="inlineStr"/>
+      <c r="Y21" t="n">
+        <v>0</v>
+      </c>
       <c r="Z21" t="inlineStr"/>
-      <c r="AA21" t="inlineStr"/>
+      <c r="AA21" t="n">
+        <v>0.114485813726807</v>
+      </c>
       <c r="AB21" t="inlineStr"/>
-      <c r="AC21" t="inlineStr"/>
+      <c r="AC21" t="n">
+        <v>0.2435606414322798</v>
+      </c>
+      <c r="AD21" t="inlineStr"/>
+      <c r="AE21" t="n">
+        <v>0.148839083264092</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>0.079358646518538</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>0.084589254540941</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2016,25 +2164,25 @@
         <v>103.1</v>
       </c>
       <c r="E22" t="n">
-        <v>4.826633115575961</v>
+        <v>4.826633115573237</v>
       </c>
       <c r="F22" t="n">
-        <v>0.4979383117367246</v>
+        <v>0.497938311736443</v>
       </c>
       <c r="G22" t="n">
-        <v>-5.547262026771099</v>
+        <v>-5.547262026771105</v>
       </c>
       <c r="H22" t="n">
-        <v>1.857080350518766</v>
+        <v>13.02677031492596</v>
       </c>
       <c r="I22" t="n">
-        <v>0.08045217911760719</v>
+        <v>0.564343949042156</v>
       </c>
       <c r="J22" t="n">
         <v>-13.21</v>
       </c>
       <c r="K22" t="n">
-        <v>0.1615705745496939</v>
+        <v>1.133361172941562</v>
       </c>
       <c r="L22" t="n">
         <v>0.13</v>
@@ -2062,12 +2210,16 @@
       </c>
       <c r="Z22" t="inlineStr"/>
       <c r="AA22" t="n">
-        <v>1.857080350518766</v>
+        <v>13.02677031492596</v>
       </c>
       <c r="AB22" t="inlineStr"/>
       <c r="AC22" t="n">
-        <v>0.08045217911760719</v>
-      </c>
+        <v>0.564343949042156</v>
+      </c>
+      <c r="AD22" t="inlineStr"/>
+      <c r="AE22" t="inlineStr"/>
+      <c r="AF22" t="inlineStr"/>
+      <c r="AG22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2089,25 +2241,25 @@
         <v>329.4</v>
       </c>
       <c r="E23" t="n">
-        <v>2.511143874209221</v>
+        <v>2.511143874209327</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3475710873792958</v>
+        <v>0.3475710873793104</v>
       </c>
       <c r="G23" t="n">
         <v>-13.21</v>
       </c>
       <c r="H23" t="n">
-        <v>0.352280009908192</v>
+        <v>2.173506696494945</v>
       </c>
       <c r="I23" t="n">
-        <v>0.04875959014667667</v>
+        <v>0.3008382330004192</v>
       </c>
       <c r="J23" t="n">
         <v>-13.21</v>
       </c>
       <c r="K23" t="n">
-        <v>0.1402866691655124</v>
+        <v>0.8655444711145067</v>
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
@@ -2133,12 +2285,16 @@
       </c>
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="n">
-        <v>0.352280009908192</v>
+        <v>2.173506696494945</v>
       </c>
       <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="n">
-        <v>0.04875959014667667</v>
-      </c>
+        <v>0.3008382330004192</v>
+      </c>
+      <c r="AD23" t="inlineStr"/>
+      <c r="AE23" t="inlineStr"/>
+      <c r="AF23" t="inlineStr"/>
+      <c r="AG23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2160,25 +2316,25 @@
         <v>228.24</v>
       </c>
       <c r="E24" t="n">
-        <v>1.465955758988965</v>
+        <v>1.465955759336204</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3345898405304225</v>
+        <v>0.3345898406096754</v>
       </c>
       <c r="G24" t="n">
-        <v>-5.550743282537618</v>
+        <v>-5.550743282537632</v>
       </c>
       <c r="H24" t="n">
-        <v>0.509380836314185</v>
+        <v>3.857755474743915</v>
       </c>
       <c r="I24" t="n">
-        <v>0.04885205220172191</v>
+        <v>0.3699771534346199</v>
       </c>
       <c r="J24" t="n">
         <v>-13.21</v>
       </c>
       <c r="K24" t="n">
-        <v>0.1460057846474871</v>
+        <v>1.105763261551705</v>
       </c>
       <c r="L24" t="n">
         <v>0.0002</v>
@@ -2206,12 +2362,16 @@
       </c>
       <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="n">
-        <v>0.509380836314185</v>
+        <v>3.857755474743915</v>
       </c>
       <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="n">
-        <v>0.04885205220172191</v>
-      </c>
+        <v>0.3699771534346199</v>
+      </c>
+      <c r="AD24" t="inlineStr"/>
+      <c r="AE24" t="inlineStr"/>
+      <c r="AF24" t="inlineStr"/>
+      <c r="AG24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2233,25 +2393,25 @@
         <v>246.3</v>
       </c>
       <c r="E25" t="n">
-        <v>1.116107088093233</v>
+        <v>1.116107087963434</v>
       </c>
       <c r="F25" t="n">
-        <v>0.2748980962445054</v>
+        <v>0.274898096212535</v>
       </c>
       <c r="G25" t="n">
-        <v>-5.550726324289684</v>
+        <v>-5.550726324289699</v>
       </c>
       <c r="H25" t="n">
-        <v>0.335248349762481</v>
+        <v>2.848944201796989</v>
       </c>
       <c r="I25" t="n">
-        <v>0.03469600824314574</v>
+        <v>0.2948470636166959</v>
       </c>
       <c r="J25" t="n">
         <v>-13.21</v>
       </c>
       <c r="K25" t="n">
-        <v>0.1262140724768269</v>
+        <v>1.072568590612347</v>
       </c>
       <c r="L25" t="n">
         <v>0.003</v>
@@ -2279,12 +2439,16 @@
       </c>
       <c r="Z25" t="inlineStr"/>
       <c r="AA25" t="n">
-        <v>0.335248349762481</v>
+        <v>2.848944201796989</v>
       </c>
       <c r="AB25" t="inlineStr"/>
       <c r="AC25" t="n">
-        <v>0.03469600824314574</v>
-      </c>
+        <v>0.2948470636166959</v>
+      </c>
+      <c r="AD25" t="inlineStr"/>
+      <c r="AE25" t="inlineStr"/>
+      <c r="AF25" t="inlineStr"/>
+      <c r="AG25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2306,25 +2470,25 @@
         <v>174.15</v>
       </c>
       <c r="E26" t="n">
-        <v>9.725652187360838</v>
+        <v>9.72565218736068</v>
       </c>
       <c r="F26" t="n">
-        <v>0.7116896739912171</v>
+        <v>0.7116896739912054</v>
       </c>
       <c r="G26" t="n">
         <v>-13.21</v>
       </c>
       <c r="H26" t="n">
-        <v>2.821654520563765</v>
+        <v>9.705902615627961</v>
       </c>
       <c r="I26" t="n">
-        <v>0.2064789432286701</v>
+        <v>0.7102444684669743</v>
       </c>
       <c r="J26" t="n">
         <v>-13.21</v>
       </c>
       <c r="K26" t="n">
-        <v>0.2901249670670623</v>
+        <v>0.9979693318913477</v>
       </c>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
@@ -2350,12 +2514,16 @@
       </c>
       <c r="Z26" t="inlineStr"/>
       <c r="AA26" t="n">
-        <v>2.821654520563765</v>
+        <v>9.705902615627961</v>
       </c>
       <c r="AB26" t="inlineStr"/>
       <c r="AC26" t="n">
-        <v>0.2064789432286701</v>
-      </c>
+        <v>0.7102444684669743</v>
+      </c>
+      <c r="AD26" t="inlineStr"/>
+      <c r="AE26" t="inlineStr"/>
+      <c r="AF26" t="inlineStr"/>
+      <c r="AG26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2385,10 +2553,18 @@
       <c r="G27" t="n">
         <v>-0.332925</v>
       </c>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr"/>
+      <c r="H27" t="n">
+        <v>0.101731147348485</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.241475108861812</v>
+      </c>
+      <c r="J27" t="n">
+        <v>-0.332925</v>
+      </c>
+      <c r="K27" t="n">
+        <v>1.003309403104896</v>
+      </c>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr">
@@ -2402,15 +2578,35 @@
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
-      <c r="U27" t="inlineStr"/>
+      <c r="U27" t="n">
+        <v>0.15276519020913</v>
+      </c>
       <c r="V27" t="inlineStr"/>
-      <c r="W27" t="inlineStr"/>
+      <c r="W27" t="n">
+        <v>-0.332925</v>
+      </c>
       <c r="X27" t="inlineStr"/>
-      <c r="Y27" t="inlineStr"/>
+      <c r="Y27" t="n">
+        <v>0</v>
+      </c>
       <c r="Z27" t="inlineStr"/>
-      <c r="AA27" t="inlineStr"/>
+      <c r="AA27" t="n">
+        <v>0.101731147348485</v>
+      </c>
       <c r="AB27" t="inlineStr"/>
-      <c r="AC27" t="inlineStr"/>
+      <c r="AC27" t="n">
+        <v>0.241475108861812</v>
+      </c>
+      <c r="AD27" t="inlineStr"/>
+      <c r="AE27" t="n">
+        <v>0.153175639705909</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>0.078807086651177</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>0.08371505342808699</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2432,25 +2628,25 @@
         <v>104.15</v>
       </c>
       <c r="E28" t="n">
-        <v>2.49154977966135</v>
+        <v>2.491549779661428</v>
       </c>
       <c r="F28" t="n">
-        <v>0.2594955560978252</v>
+        <v>0.2594955560978311</v>
       </c>
       <c r="G28" t="n">
-        <v>-5.550731080009659</v>
+        <v>-5.550731080009707</v>
       </c>
       <c r="H28" t="n">
-        <v>1.803759699499738</v>
+        <v>6.737144784561575</v>
       </c>
       <c r="I28" t="n">
-        <v>0.07893805211650186</v>
+        <v>0.2948381019199157</v>
       </c>
       <c r="J28" t="n">
         <v>-13.21</v>
       </c>
       <c r="K28" t="n">
-        <v>0.3041980884125184</v>
+        <v>1.136197113945027</v>
       </c>
       <c r="L28" t="n">
         <v>0.001</v>
@@ -2478,12 +2674,16 @@
       </c>
       <c r="Z28" t="inlineStr"/>
       <c r="AA28" t="n">
-        <v>1.803759699499738</v>
+        <v>6.737144784561575</v>
       </c>
       <c r="AB28" t="inlineStr"/>
       <c r="AC28" t="n">
-        <v>0.07893805211650186</v>
-      </c>
+        <v>0.2948381019199157</v>
+      </c>
+      <c r="AD28" t="inlineStr"/>
+      <c r="AE28" t="inlineStr"/>
+      <c r="AF28" t="inlineStr"/>
+      <c r="AG28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2514,16 +2714,16 @@
         <v>-2.20113372715757</v>
       </c>
       <c r="H29" t="n">
-        <v>0.01090964555087</v>
+        <v>0.129384562314843</v>
       </c>
       <c r="I29" t="n">
-        <v>0.02267780783519924</v>
+        <v>0.2689508313845617</v>
       </c>
       <c r="J29" t="n">
         <v>-2.201133727157571</v>
       </c>
       <c r="K29" t="n">
-        <v>0.08338008990721182</v>
+        <v>0.9888585644798107</v>
       </c>
       <c r="L29" t="n">
         <v>0.14</v>
@@ -2555,12 +2755,16 @@
       </c>
       <c r="Z29" t="inlineStr"/>
       <c r="AA29" t="n">
-        <v>0.01090964555087</v>
+        <v>0.129384562314843</v>
       </c>
       <c r="AB29" t="inlineStr"/>
       <c r="AC29" t="n">
-        <v>0.02267780783519924</v>
-      </c>
+        <v>0.2689508313845617</v>
+      </c>
+      <c r="AD29" t="inlineStr"/>
+      <c r="AE29" t="inlineStr"/>
+      <c r="AF29" t="inlineStr"/>
+      <c r="AG29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2616,6 +2820,10 @@
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="inlineStr"/>
       <c r="AC30" t="inlineStr"/>
+      <c r="AD30" t="inlineStr"/>
+      <c r="AE30" t="inlineStr"/>
+      <c r="AF30" t="inlineStr"/>
+      <c r="AG30" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>